<commit_message>
Update styles and database operations
</commit_message>
<xml_diff>
--- a/IA1.xlsx
+++ b/IA1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Project\TGMS_System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Project\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,57 +33,30 @@
     <t>Ansari Taha Mohd Javed</t>
   </si>
   <si>
-    <t>2021HE0284</t>
-  </si>
-  <si>
     <t>Bachkar Harsh Ramdas</t>
   </si>
   <si>
-    <t>2021HE0664</t>
-  </si>
-  <si>
     <t>Balwal Dhruv Madan Gopal</t>
   </si>
   <si>
-    <t>2021HE0544</t>
-  </si>
-  <si>
     <t>Betkar Ritesh Tukaram</t>
   </si>
   <si>
-    <t>2021HE0553</t>
-  </si>
-  <si>
     <t>Bhoir Kaustubh Sanjiv</t>
   </si>
   <si>
-    <t>2021HE0653</t>
-  </si>
-  <si>
     <t>Bhopale Aditi Vivekanand</t>
   </si>
   <si>
-    <t>2021HE0583</t>
-  </si>
-  <si>
     <t>Bhosale Aryan Sandeep</t>
   </si>
   <si>
-    <t>2021HE0523</t>
-  </si>
-  <si>
     <t>Borude Ashutosh Kanifnath</t>
   </si>
   <si>
-    <t>2021HE0661</t>
-  </si>
-  <si>
     <t>Chander Mohit Sharma Romesh</t>
   </si>
   <si>
-    <t>2021HE0431</t>
-  </si>
-  <si>
     <t>Chavre Shruti Shashikant</t>
   </si>
   <si>
@@ -118,6 +91,33 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>2021HE0573</t>
+  </si>
+  <si>
+    <t>2021HE0574</t>
+  </si>
+  <si>
+    <t>2021HE0575</t>
+  </si>
+  <si>
+    <t>2021HE0576</t>
+  </si>
+  <si>
+    <t>2021HE0577</t>
+  </si>
+  <si>
+    <t>2021HE0578</t>
+  </si>
+  <si>
+    <t>2021HE0579</t>
+  </si>
+  <si>
+    <t>2021HE0580</t>
+  </si>
+  <si>
+    <t>2021HE0581</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -511,31 +511,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -564,7 +564,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="5">
-        <f>(D2+E2+G2+F2+H2)</f>
+        <f t="shared" ref="I2:I12" si="0">(D2+E2+G2+F2+H2)</f>
         <v>68</v>
       </c>
     </row>
@@ -573,10 +573,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="D3" s="5">
         <v>8</v>
@@ -594,7 +594,7 @@
         <v>15</v>
       </c>
       <c r="I3" s="5">
-        <f>(D3+E3+G3+F3+H3)</f>
+        <f t="shared" si="0"/>
         <v>61</v>
       </c>
     </row>
@@ -603,10 +603,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="5">
         <v>15</v>
@@ -624,7 +624,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="5">
-        <f>(D4+E4+G4+F4+H4)</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
@@ -633,10 +633,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5">
         <v>14</v>
@@ -654,7 +654,7 @@
         <v>11</v>
       </c>
       <c r="I5" s="5">
-        <f>(D5+E5+G5+F5+H5)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
     </row>
@@ -663,10 +663,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D6" s="5">
         <v>16</v>
@@ -684,7 +684,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="5">
-        <f>(D6+E6+G6+F6+H6)</f>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
@@ -693,10 +693,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5">
         <v>17</v>
@@ -714,7 +714,7 @@
         <v>7</v>
       </c>
       <c r="I7" s="5">
-        <f>(D7+E7+G7+F7+H7)</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
@@ -723,10 +723,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5">
         <v>15</v>
@@ -744,7 +744,7 @@
         <v>15</v>
       </c>
       <c r="I8" s="5">
-        <f>(D8+E8+G8+F8+H8)</f>
+        <f t="shared" si="0"/>
         <v>78</v>
       </c>
     </row>
@@ -753,10 +753,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D9" s="5">
         <v>14</v>
@@ -774,7 +774,7 @@
         <v>11</v>
       </c>
       <c r="I9" s="5">
-        <f>(D9+E9+G9+F9+H9)</f>
+        <f t="shared" si="0"/>
         <v>75</v>
       </c>
     </row>
@@ -783,10 +783,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5">
         <v>16</v>
@@ -804,7 +804,7 @@
         <v>10</v>
       </c>
       <c r="I10" s="5">
-        <f>(D10+E10+G10+F10+H10)</f>
+        <f t="shared" si="0"/>
         <v>69</v>
       </c>
     </row>
@@ -813,10 +813,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D11" s="5">
         <v>17</v>
@@ -834,7 +834,7 @@
         <v>7</v>
       </c>
       <c r="I11" s="5">
-        <f>(D11+E11+G11+F11+H11)</f>
+        <f t="shared" si="0"/>
         <v>79</v>
       </c>
     </row>
@@ -843,10 +843,10 @@
         <v>63</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D12" s="5">
         <v>14</v>
@@ -864,7 +864,7 @@
         <v>7</v>
       </c>
       <c r="I12" s="5">
-        <f>(D12+E12+G12+F12+H12)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
     </row>

</xml_diff>